<commit_message>
Changelog: - First objects for ProjectCostCalculation implemented - Some amounts in the job-detail view were wrong and are now fixed (verified_amount was replaced by amount_a_reductions) - job_additions have an additional field (name) - invoice check is now created only once and then copied
</commit_message>
<xml_diff>
--- a/templates/invoice_check.xlsx
+++ b/templates/invoice_check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Eigene Dateien\Google Drive\02 Arbeit\00 Fyuture\01 Learning\Python\00 Projekte\Kostenfortschreibung\Application\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788D5039-A3A4-47F4-BDC8-3F22980647A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CE3481-03FD-4AFF-82A9-E1E772E3F300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-4995" windowWidth="29040" windowHeight="15840" xr2:uid="{22F6EF0F-DCEC-4D99-A842-747235C2D3BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{22F6EF0F-DCEC-4D99-A842-747235C2D3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -200,10 +200,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0%;0%;&quot;-&quot;"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -491,9 +492,6 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -585,6 +583,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
@@ -960,8 +961,8 @@
   </sheetPr>
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,11 +970,11 @@
     <col min="1" max="1" width="4.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="5.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="57" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="56" customWidth="1"/>
     <col min="5" max="5" width="8" style="4" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" style="53" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" style="52" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="18.140625" style="4" customWidth="1"/>
     <col min="11" max="11" width="24.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -1005,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="58"/>
+      <c r="D2" s="57"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1018,11 +1019,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" s="59"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="54"/>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1032,7 +1033,7 @@
       <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="59" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="11" t="s">
@@ -1046,162 +1047,162 @@
       <c r="C8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="H8" s="55" t="s">
+      <c r="D8" s="59"/>
+      <c r="H8" s="54" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="46" t="s">
+      <c r="D11" s="73"/>
+      <c r="E11" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="45" t="s">
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="44" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="30" t="s">
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="73"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="12"/>
-      <c r="D14" s="57" t="s">
+      <c r="D14" s="56" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="53" t="s">
+      <c r="H14" s="52" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="12"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="38"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="38"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="12"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="38"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="12"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
-      <c r="D18" s="61"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="75"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="74"/>
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="12"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="38"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="12"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="38"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="37"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="12"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="38"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="37"/>
       <c r="I21" s="12"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="12"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="38"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="12"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="38"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="37"/>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="12"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="48"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="12"/>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="43"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44" t="s">
+      <c r="C25" s="42"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="70" t="s">
+      <c r="G25" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="H25" s="29" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="63"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="27" t="s">
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="26" t="s">
         <v>30</v>
       </c>
       <c r="J26" s="15"/>
@@ -1210,37 +1211,37 @@
       <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="57" t="s">
+      <c r="D27" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="28" t="s">
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="27" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="64"/>
+      <c r="D28" s="63"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="31" t="s">
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="17"/>
-      <c r="D29" s="65"/>
+      <c r="D29" s="64"/>
       <c r="H29" s="18"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="66"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1250,77 +1251,77 @@
       <c r="C31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="47"/>
-      <c r="H31" s="28" t="s">
+      <c r="G31" s="46"/>
+      <c r="H31" s="27" t="s">
         <v>39</v>
       </c>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="67"/>
+      <c r="D32" s="66"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
-      <c r="H32" s="24" t="s">
+      <c r="H32" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="68"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="56" t="s">
+      <c r="D34" s="67"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="33" t="s">
+      <c r="G34" s="33"/>
+      <c r="H34" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="69"/>
-      <c r="E35" s="35" t="s">
+      <c r="D35" s="68"/>
+      <c r="E35" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32" t="s">
+      <c r="F35" s="39"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31" t="s">
         <v>37</v>
       </c>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="68"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="56" t="s">
+      <c r="D36" s="67"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="34"/>
-      <c r="H36" s="33" t="s">
+      <c r="G36" s="33"/>
+      <c r="H36" s="32" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="22" t="s">
+      <c r="C39" s="39"/>
+      <c r="D39" s="21" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>